<commit_message>
Preparing Management Process module
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>url</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>CourseIntro</t>
+  </si>
+  <si>
+    <t>ManagementProcess</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,6 +531,12 @@
         <f>C3+2</f>
         <v>44581</v>
       </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -897,19 +906,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A2:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Starting Management Tools module
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>url</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>ManagementProcess</t>
+  </si>
+  <si>
+    <t>ManagementTools</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,6 +552,12 @@
         <f>C4+5</f>
         <v>44586</v>
       </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -908,7 +917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
More work on Management Tools
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,6 +570,9 @@
         <f>C5+2</f>
         <v>44588</v>
       </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -918,7 +921,7 @@
   <dimension ref="A2:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,11 +931,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Started work on SizeStructure1
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>url</t>
   </si>
@@ -165,9 +165,6 @@
     <t>WeightLength</t>
   </si>
   <si>
-    <t>SizeStructure</t>
-  </si>
-  <si>
     <t>BagLimits</t>
   </si>
   <si>
@@ -190,6 +187,18 @@
   </si>
   <si>
     <t>Mortality I</t>
+  </si>
+  <si>
+    <t>Size Structure I</t>
+  </si>
+  <si>
+    <t>SizeStructure1</t>
+  </si>
+  <si>
+    <t>Size Structure II</t>
+  </si>
+  <si>
+    <t>SizeStructure2</t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +676,7 @@
         <v>44595</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -757,10 +766,10 @@
         <v>44614</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -775,10 +784,10 @@
         <v>44616</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -853,10 +862,10 @@
         <v>44635</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -871,10 +880,10 @@
         <v>44637</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -889,10 +898,10 @@
         <v>44642</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -907,10 +916,10 @@
         <v>44644</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -925,10 +934,10 @@
         <v>44649</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,10 +952,10 @@
         <v>44651</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -961,10 +970,10 @@
         <v>44656</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -989,6 +998,12 @@
       <c r="C27" s="1">
         <f>C26+5</f>
         <v>44663</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Working on Getting Organized
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>url</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Midterm Exam</t>
+  </si>
+  <si>
+    <t>GetOrganized</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,6 +581,9 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More mortality prep work
</commit_message>
<xml_diff>
--- a/resources/Dates_349.xlsx
+++ b/resources/Dates_349.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>url</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>GetOrganized</t>
+  </si>
+  <si>
+    <t>MT1</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,6 +818,9 @@
       </c>
       <c r="D15" t="s">
         <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>